<commit_message>
Import tmt test cases from remote repositories. E2E Testing for Sw Requirement imports and Test Case import
Signed-off-by: Luigi Pellecchia <lpellecc@redhat.com>
</commit_message>
<xml_diff>
--- a/examples/import/reqs/reqs.xlsx
+++ b/examples/import/reqs/reqs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
   <si>
     <t>Tabella 1</t>
   </si>
@@ -41,6 +41,18 @@
   </si>
   <si>
     <t>Software requirement description three</t>
+  </si>
+  <si>
+    <t>req4</t>
+  </si>
+  <si>
+    <t>Software requirement description four</t>
+  </si>
+  <si>
+    <t>req5</t>
+  </si>
+  <si>
+    <t>Software requirement description five</t>
   </si>
 </sst>
 </file>
@@ -1413,18 +1425,30 @@
     </row>
     <row r="6" ht="20.05" customHeight="1">
       <c r="A6" s="9"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
+      <c r="B6" s="10">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s" s="11">
+        <v>11</v>
+      </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" s="9"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="B7" s="10">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s" s="11">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s" s="11">
+        <v>13</v>
+      </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>

</xml_diff>

<commit_message>
Import tmt test cases from remote repositories (#110)
* Import tmt test cases from remote repositories. E2E Testing for Sw Requirement imports and Test Case import

Signed-off-by: Luigi Pellecchia <lpellecc@redhat.com>

* Update import_test_case.cy.js

wait 2 minutes after requesting the json creation

* Fix import test case test, need to click the refresh user files list before searching for an entry there

Signed-off-by: Luigi Pellecchia <lpellecc@redhat.com>

* Update build.yaml

Upload cypress screenshots in case of failure

* Add wait after loading test cases from user files

Signed-off-by: Luigi Pellecchia <lpellecc@redhat.com>

* Update build.yaml

Add user-files to the uploaded artifacts in case of failure of cypress testing

* Add jq package in the api images requirements

Signed-off-by: Luigi Pellecchia <lpellecc@redhat.com>

---------

Signed-off-by: Luigi Pellecchia <lpellecc@redhat.com>
Co-authored-by: Luigi Pellecchia <lpellecc@redhat.com>
</commit_message>
<xml_diff>
--- a/examples/import/reqs/reqs.xlsx
+++ b/examples/import/reqs/reqs.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
   <si>
     <t>Tabella 1</t>
   </si>
@@ -41,6 +41,18 @@
   </si>
   <si>
     <t>Software requirement description three</t>
+  </si>
+  <si>
+    <t>req4</t>
+  </si>
+  <si>
+    <t>Software requirement description four</t>
+  </si>
+  <si>
+    <t>req5</t>
+  </si>
+  <si>
+    <t>Software requirement description five</t>
   </si>
 </sst>
 </file>
@@ -1413,18 +1425,30 @@
     </row>
     <row r="6" ht="20.05" customHeight="1">
       <c r="A6" s="9"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
+      <c r="B6" s="10">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s" s="11">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s" s="11">
+        <v>11</v>
+      </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
       <c r="A7" s="9"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="B7" s="10">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s" s="11">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s" s="11">
+        <v>13</v>
+      </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>

</xml_diff>